<commit_message>
Små bug-fix og bedre print
</commit_message>
<xml_diff>
--- a/simulation/PythonEksport.xlsx
+++ b/simulation/PythonEksport.xlsx
@@ -1,63 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinesorli/Chris-Tora-master/simulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinehagen/PycharmProjects/chris/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A930B3-62A9-B944-BF51-B990FA682AAC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14200"/>
+    <workbookView xWindow="220" yWindow="1100" windowWidth="32460" windowHeight="18380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ett produkt av gangen" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
-  <si>
-    <t>Scenario</t>
-  </si>
-  <si>
-    <t>(Antall bokser)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Day </t>
-  </si>
-  <si>
-    <t>Profit</t>
-  </si>
-  <si>
-    <t>Internal (x)</t>
-  </si>
-  <si>
-    <t>External (y)</t>
-  </si>
-  <si>
-    <t>Sum</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Hvor mye dårligere blir modellen dersom vi må optimere for ett produkt av gangen? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Felles for alle kjøringene: </t>
+  </si>
+  <si>
+    <t>Solution method</t>
+  </si>
+  <si>
+    <t>Deterministisk</t>
+  </si>
+  <si>
+    <t>Number of days</t>
+  </si>
+  <si>
+    <t>One product at the time</t>
+  </si>
+  <si>
+    <t>Start day</t>
+  </si>
+  <si>
+    <t>Run Time</t>
+  </si>
+  <si>
+    <t>Objective function</t>
+  </si>
+  <si>
+    <t>Change in objective function</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hvorfor er det interessant? </t>
+  </si>
+  <si>
+    <t>Fordi vi må ta ett produkt av gangen når vi bruker stokastiske, og derfor er vi interessert i å se hvor mye kvalitet vi minster. Siden vi ikke kan teste med alle produkter på en gang med den stokastiske, må denne testen gjøres med den deterministiske</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hvordan testet: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Når vi kjører med ett produkt av gangen fjerner vi cross docking fra objektivet. I stedenfor blir cross docking-kostnaden regnet ut etter at alle produktene er optimert. </t>
+  </si>
+  <si>
+    <t>Har testet med tre forskjellige uker for å få mer riktig resultat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resultat: </t>
+  </si>
+  <si>
+    <t>Vi ser at objektivverdien blir i gjennomsnitt 1,07  % dårligere</t>
+  </si>
+  <si>
+    <t>Stokastisk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-[$kr-414]\ * #,##0.00_-;\-[$kr-414]\ * #,##0.00_-;_-[$kr-414]\ * &quot;-&quot;??_-;_-@_-"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,16 +114,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -90,67 +152,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Prosent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -452,160 +479,281 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.83203125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3.6</v>
+      </c>
+      <c r="D11">
+        <v>32731907</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+      <c r="D12">
+        <v>32346582</v>
+      </c>
+      <c r="E12" s="2">
+        <f>(D12-D11)/D11</f>
+        <v>-1.1772152474953567E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>8.66</v>
+      </c>
+      <c r="D13">
+        <v>56022018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>0.6</v>
+      </c>
+      <c r="D14">
+        <v>55013815</v>
+      </c>
+      <c r="E14" s="2">
+        <f>(D14-D13)/D13</f>
+        <v>-1.7996549142517502E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>2.27</v>
+      </c>
+      <c r="D15">
+        <v>23419078</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>0.3</v>
+      </c>
+      <c r="D16">
+        <v>23363780</v>
+      </c>
+      <c r="E16" s="2">
+        <f>(D16-D15)/D15</f>
+        <v>-2.361237278427443E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="6">
+        <f>AVERAGE(E12,E14,E16)</f>
+        <v>-1.070997963196617E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A7:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="16.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" style="9" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="G2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="E7">
+        <v>8.15</v>
+      </c>
+      <c r="F7">
+        <v>18295492</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="E8">
+        <v>3.9</v>
+      </c>
+      <c r="F8">
+        <v>24649578</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="E4" s="7">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="E5" s="7">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="E6" s="7">
-        <v>3</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>4</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="E7" s="7">
-        <v>4</v>
-      </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>5</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="E8" s="7">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="E9" s="7">
-        <v>6</v>
-      </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="E10" s="7">
-        <v>7</v>
-      </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="2"/>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>4.88</v>
+      </c>
+      <c r="F9">
+        <v>36987694</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:H2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Results from one run testing
</commit_message>
<xml_diff>
--- a/simulation/PythonEksport.xlsx
+++ b/simulation/PythonEksport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinehagen/PycharmProjects/chris/simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3059CEF0-BF9B-1C43-846C-6148F346C529}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9C8547-71F8-2844-A79B-75E91E9313D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EEV osv" sheetId="19" r:id="rId1"/>
@@ -639,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC7916F0-0759-E240-9EE4-4F14444A795E}">
   <dimension ref="A5:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:BQ148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -57204,8 +57204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:CU146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="I144" sqref="I144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -61744,6 +61744,10 @@
       </c>
       <c r="B26">
         <v>1.6059853076934809</v>
+      </c>
+      <c r="H26">
+        <f>AVERAGE(H10:H24)</f>
+        <v>31894.400000000001</v>
       </c>
       <c r="K26" t="s">
         <v>40</v>
@@ -75634,6 +75638,12 @@
       </c>
       <c r="CN139">
         <v>8.4620426019032795</v>
+      </c>
+    </row>
+    <row r="140" spans="1:99" x14ac:dyDescent="0.2">
+      <c r="H140">
+        <f>AVERAGE(H123:H137)</f>
+        <v>86772.4</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>